<commit_message>
Updated Invoice New Format
</commit_message>
<xml_diff>
--- a/PENDING_TASK/AFTER JUDGMENT PROCEEDINGS.xlsx
+++ b/PENDING_TASK/AFTER JUDGMENT PROCEEDINGS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive_account\OneDrive - Yands LLC\NEW SISTEM UPDATE\التدقيق بعد التحديث بكره\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working\Git\a4aliadnan@gmail.com\LMS\PENDING_TASK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEC580F-2B5F-4D95-AA95-6907EFA980B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F89585C-2F95-4AA1-8C30-734027A05F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3A937E9C-6024-470C-8151-A61C2F387E10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3A937E9C-6024-470C-8151-A61C2F387E10}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -308,8 +308,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>212912</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>134472</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -324,8 +324,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3630705" y="1154207"/>
-          <a:ext cx="2734236" cy="773206"/>
+          <a:off x="3238499" y="1221442"/>
+          <a:ext cx="2420472" cy="1434352"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4363,10 +4363,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4378,10 +4378,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4392,15 +4392,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D38FB8-515B-4124-AC4F-CA92D3C86A8F}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4415,7 +4415,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4430,7 +4430,7 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4445,7 +4445,7 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4456,11 +4456,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA436AF-083A-46E3-A64A-A1B9C1144AF3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>